<commit_message>
First execution with final data
</commit_message>
<xml_diff>
--- a/Data/HighFuel/OPEX.xlsx
+++ b/Data/HighFuel/OPEX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee65a08843967445/Desktop/Master Ordner Konsti/03_Studium/Master/Sustainable Energy - Energy Systems Analysis/Masterarbeit/MasterThesis/Data/HighFuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{62F7584F-92F1-43AB-8684-75104CC73B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C615DF82-E01A-4971-939B-E55A3EC78A3F}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{62F7584F-92F1-43AB-8684-75104CC73B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2F6E7DE-0205-4C74-9651-709F5C628A12}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{A6326503-DCBD-45B8-99ED-538B88B01DFC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A6326503-DCBD-45B8-99ED-538B88B01DFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Technology</t>
   </si>
@@ -74,9 +74,6 @@
     <t>CO2 Price [€/t]</t>
   </si>
   <si>
-    <t>Operating Cost</t>
-  </si>
-  <si>
     <t>Gas</t>
   </si>
   <si>
@@ -96,12 +93,37 @@
   </si>
   <si>
     <t>CO2 emissions [t/MWh]</t>
+  </si>
+  <si>
+    <t>Fixed OPEX [EUR/kW]</t>
+  </si>
+  <si>
+    <t>Fixed OPEX [EUR/GW]</t>
+  </si>
+  <si>
+    <t>Variable OPEX [EUR/kWh]</t>
+  </si>
+  <si>
+    <t>Variable OPEX [EUR/MWh]</t>
+  </si>
+  <si>
+    <t>Total OPEX [€/MWh]</t>
+  </si>
+  <si>
+    <t>Carbon cost [€/MWh]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,16 +157,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -478,348 +512,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3C0376-C367-490E-9900-8B92DE61B264}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="32.81640625" customWidth="1"/>
+    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="B2">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3">
+        <f>B2*1000000</f>
+        <v>39000000</v>
+      </c>
+      <c r="D2" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2*1000</f>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <f>C2/D2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>150</v>
-      </c>
-      <c r="H2">
-        <f>(E2+F2*G2)*1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H2" s="11">
+        <f>F2/G2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>180</v>
+      </c>
+      <c r="K2" s="1">
+        <f>J2*I2</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" ref="L2:L13" si="0">(H2+I2*J2+E2)</f>
+        <v>7</v>
+      </c>
+      <c r="M2" s="3">
+        <f>(H2+I2*J2+E2)*1000</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="B3">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ref="C3:C13" si="1">B3*1000000</f>
+        <v>32000000</v>
+      </c>
+      <c r="D3" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E13" si="2">D3*1000</f>
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E13" si="0">C3/D3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>150</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H13" si="1">(E3+F3*G3)*1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H3" s="11">
+        <f t="shared" ref="H3:H13" si="3">F3/G3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>180</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K13" si="4">J3*I3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M13" si="5">(H3+I3*J3+E3)*1000</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="B4">
+        <f>4631*0.04</f>
+        <v>185.24</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="1"/>
+        <v>185240000</v>
+      </c>
+      <c r="D4" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F4">
         <v>25.5</v>
       </c>
-      <c r="D4">
+      <c r="G4">
         <v>0.32700000000000001</v>
       </c>
-      <c r="E4" s="2">
-        <f>C4/D4</f>
+      <c r="H4" s="11">
+        <f>F4/G4</f>
         <v>77.981651376146786</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>150</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>77981.65137614678</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>180</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="0"/>
+        <v>81.981651376146786</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="5"/>
+        <v>81981.65137614678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>42000000</v>
+      </c>
+      <c r="D5" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F5">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <v>0.39</v>
       </c>
-      <c r="E5" s="2">
+      <c r="H5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.8974358974358969</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="J5" s="1">
+        <v>180</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="4"/>
+        <v>188.82</v>
+      </c>
+      <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>5.8974358974358969</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.0489999999999999</v>
-      </c>
-      <c r="G5" s="1">
-        <v>150</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>163247.43589743588</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>199.71743589743588</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="5"/>
+        <v>199717.43589743588</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="B6">
+        <v>37</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="1"/>
+        <v>37000000</v>
+      </c>
+      <c r="D6" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F6">
         <v>11.6</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>0.4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="H6" s="12">
+        <f>F6/G6</f>
+        <v>28.999999999999996</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="J6" s="1">
+        <v>180</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="4"/>
+        <v>156.06</v>
+      </c>
+      <c r="L6" s="9">
         <f t="shared" si="0"/>
-        <v>28.999999999999996</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="G6" s="1">
+        <v>190.06</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="5"/>
+        <v>190060</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>21.5</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="1"/>
+        <v>21500000</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="F7">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="J7" s="1">
+        <v>180</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="4"/>
+        <v>64.44</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="0"/>
+        <v>122.94</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="5"/>
+        <v>122940</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="1"/>
+        <v>24000000</v>
+      </c>
+      <c r="D8" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F8">
         <v>150</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>159050</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <v>27</v>
-      </c>
-      <c r="D7">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>180</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L8" s="9">
         <f t="shared" si="0"/>
-        <v>67.5</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="G7" s="1">
-        <v>150</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>121199.99999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-      <c r="D8">
-        <v>0.4</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>375</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>150</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>375000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="5"/>
+        <v>305000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="1"/>
+        <v>100000000</v>
+      </c>
+      <c r="D9" s="7">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F9">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>0.35</v>
       </c>
-      <c r="E9" s="2">
+      <c r="H9" s="12">
+        <f t="shared" si="3"/>
+        <v>22.857142857142858</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>180</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="9">
         <f t="shared" si="0"/>
-        <v>22.857142857142858</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>150</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>22857.142857142859</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <v>29.857142857142858</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="5"/>
+        <v>29857.142857142859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+      <c r="B10">
+        <v>13.3</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="1"/>
+        <v>13300000</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>1</v>
       </c>
-      <c r="E10" s="2">
+      <c r="H10" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>180</v>
+      </c>
+      <c r="K10" s="9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>150</v>
-      </c>
-      <c r="H10">
+      <c r="M10" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+        <v>70000000</v>
+      </c>
+      <c r="D11" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>180</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="5"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B12">
+        <v>90</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>90000000</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="H12" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>180</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>150</v>
-      </c>
-      <c r="H11">
+        <v>8</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="5"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
+        <v>22000000</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>0.4</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="I13" s="2">
+        <f>I7*(266/201)</f>
+        <v>0.47377114427860695</v>
+      </c>
+      <c r="J13" s="1">
+        <v>180</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="4"/>
+        <v>85.27880597014925</v>
+      </c>
+      <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>150</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13">
-        <v>100</v>
-      </c>
-      <c r="D13">
-        <v>0.4</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="F13" s="2">
-        <f>F7*(266/201)</f>
-        <v>0.47377114427860695</v>
-      </c>
-      <c r="G13" s="1">
-        <v>150</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>321065.67164179101</v>
+        <v>340.27880597014928</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="5"/>
+        <v>340278.80597014929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>